<commit_message>
Analysis for rep 5
</commit_message>
<xml_diff>
--- a/data/combined_individual_data.xlsx
+++ b/data/combined_individual_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jy33\OneDrive\Desktop\R\bb_soc_exp\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janya\Desktop\R\bb_soc_exp\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B1BB5FA-E44E-48DC-8195-9F0C40E500F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67156D91-4EF2-4AE5-83FF-8A6278D23FB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="37">
   <si>
     <t>replicate</t>
   </si>
@@ -147,9 +147,6 @@
   </si>
   <si>
     <t>both</t>
-  </si>
-  <si>
-    <t>isoalted</t>
   </si>
 </sst>
 </file>
@@ -473,11 +470,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R117"/>
+  <dimension ref="A1:R153"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N77" sqref="N77"/>
+      <pane ySplit="1" topLeftCell="A130" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K160" sqref="K160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4830,7 +4827,7 @@
         <v>10</v>
       </c>
       <c r="H85">
-        <f t="shared" ref="H85:H117" si="8">F85-G85</f>
+        <f t="shared" ref="H85:H116" si="8">F85-G85</f>
         <v>10</v>
       </c>
       <c r="I85">
@@ -6009,7 +6006,7 @@
         <v>30</v>
       </c>
       <c r="C114" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="D114" t="s">
         <v>36</v>
@@ -6169,6 +6166,1494 @@
       <c r="L117">
         <f t="shared" si="19"/>
         <v>17</v>
+      </c>
+    </row>
+    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>5</v>
+      </c>
+      <c r="B118" t="s">
+        <v>11</v>
+      </c>
+      <c r="C118" t="s">
+        <v>10</v>
+      </c>
+      <c r="D118">
+        <v>1</v>
+      </c>
+      <c r="E118">
+        <v>1</v>
+      </c>
+      <c r="F118">
+        <v>16</v>
+      </c>
+      <c r="G118">
+        <v>6</v>
+      </c>
+      <c r="H118">
+        <f>F118-G118</f>
+        <v>10</v>
+      </c>
+      <c r="I118">
+        <v>3</v>
+      </c>
+      <c r="J118">
+        <v>7</v>
+      </c>
+      <c r="K118">
+        <v>5</v>
+      </c>
+      <c r="L118">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>5</v>
+      </c>
+      <c r="B119" t="s">
+        <v>11</v>
+      </c>
+      <c r="C119" t="s">
+        <v>10</v>
+      </c>
+      <c r="D119">
+        <v>2</v>
+      </c>
+      <c r="E119">
+        <v>3</v>
+      </c>
+      <c r="F119">
+        <v>3</v>
+      </c>
+      <c r="G119">
+        <v>0</v>
+      </c>
+      <c r="H119">
+        <f t="shared" ref="H119:H152" si="20">F119-G119</f>
+        <v>3</v>
+      </c>
+      <c r="I119">
+        <v>0</v>
+      </c>
+      <c r="J119">
+        <v>1</v>
+      </c>
+      <c r="K119">
+        <v>0</v>
+      </c>
+      <c r="L119">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>5</v>
+      </c>
+      <c r="B120" t="s">
+        <v>11</v>
+      </c>
+      <c r="C120" t="s">
+        <v>10</v>
+      </c>
+      <c r="D120" t="s">
+        <v>36</v>
+      </c>
+      <c r="E120">
+        <f>SUM(E118:E119)</f>
+        <v>4</v>
+      </c>
+      <c r="F120">
+        <f t="shared" ref="F120:L120" si="21">SUM(F118:F119)</f>
+        <v>19</v>
+      </c>
+      <c r="G120">
+        <f t="shared" si="21"/>
+        <v>6</v>
+      </c>
+      <c r="H120">
+        <f t="shared" si="21"/>
+        <v>13</v>
+      </c>
+      <c r="I120">
+        <f t="shared" si="21"/>
+        <v>3</v>
+      </c>
+      <c r="J120">
+        <f t="shared" si="21"/>
+        <v>8</v>
+      </c>
+      <c r="K120">
+        <f t="shared" si="21"/>
+        <v>5</v>
+      </c>
+      <c r="L120">
+        <f t="shared" si="21"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>5</v>
+      </c>
+      <c r="B121" t="s">
+        <v>29</v>
+      </c>
+      <c r="C121" t="s">
+        <v>10</v>
+      </c>
+      <c r="D121">
+        <v>1</v>
+      </c>
+      <c r="E121">
+        <v>4</v>
+      </c>
+      <c r="F121">
+        <v>6</v>
+      </c>
+      <c r="G121">
+        <v>0</v>
+      </c>
+      <c r="H121">
+        <f t="shared" si="20"/>
+        <v>6</v>
+      </c>
+      <c r="I121">
+        <v>1</v>
+      </c>
+      <c r="J121">
+        <v>3</v>
+      </c>
+      <c r="K121">
+        <v>1</v>
+      </c>
+      <c r="L121">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>5</v>
+      </c>
+      <c r="B122" t="s">
+        <v>29</v>
+      </c>
+      <c r="C122" t="s">
+        <v>10</v>
+      </c>
+      <c r="D122">
+        <v>2</v>
+      </c>
+      <c r="E122">
+        <v>2</v>
+      </c>
+      <c r="F122">
+        <v>8</v>
+      </c>
+      <c r="G122">
+        <v>3</v>
+      </c>
+      <c r="H122">
+        <f t="shared" si="20"/>
+        <v>5</v>
+      </c>
+      <c r="I122">
+        <v>1</v>
+      </c>
+      <c r="J122">
+        <v>2</v>
+      </c>
+      <c r="K122">
+        <v>1</v>
+      </c>
+      <c r="L122">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>5</v>
+      </c>
+      <c r="B123" t="s">
+        <v>29</v>
+      </c>
+      <c r="C123" t="s">
+        <v>10</v>
+      </c>
+      <c r="D123" t="s">
+        <v>36</v>
+      </c>
+      <c r="E123">
+        <f>SUM(E121:E122)</f>
+        <v>6</v>
+      </c>
+      <c r="F123">
+        <f t="shared" ref="F123:L123" si="22">SUM(F121:F122)</f>
+        <v>14</v>
+      </c>
+      <c r="G123">
+        <f t="shared" si="22"/>
+        <v>3</v>
+      </c>
+      <c r="H123">
+        <f t="shared" si="22"/>
+        <v>11</v>
+      </c>
+      <c r="I123">
+        <f t="shared" si="22"/>
+        <v>2</v>
+      </c>
+      <c r="J123">
+        <f t="shared" si="22"/>
+        <v>5</v>
+      </c>
+      <c r="K123">
+        <f t="shared" si="22"/>
+        <v>2</v>
+      </c>
+      <c r="L123">
+        <f t="shared" si="22"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>5</v>
+      </c>
+      <c r="B124" t="s">
+        <v>18</v>
+      </c>
+      <c r="C124" t="s">
+        <v>19</v>
+      </c>
+      <c r="D124">
+        <v>1</v>
+      </c>
+      <c r="E124">
+        <v>4</v>
+      </c>
+      <c r="F124">
+        <v>14</v>
+      </c>
+      <c r="G124">
+        <v>1</v>
+      </c>
+      <c r="H124">
+        <f t="shared" si="20"/>
+        <v>13</v>
+      </c>
+      <c r="I124">
+        <v>1</v>
+      </c>
+      <c r="J124">
+        <v>2</v>
+      </c>
+      <c r="K124">
+        <v>11</v>
+      </c>
+      <c r="L124">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>5</v>
+      </c>
+      <c r="B125" t="s">
+        <v>18</v>
+      </c>
+      <c r="C125" t="s">
+        <v>19</v>
+      </c>
+      <c r="D125">
+        <v>2</v>
+      </c>
+      <c r="E125">
+        <v>0</v>
+      </c>
+      <c r="F125">
+        <v>2</v>
+      </c>
+      <c r="G125">
+        <v>1</v>
+      </c>
+      <c r="H125">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+      <c r="I125">
+        <v>0</v>
+      </c>
+      <c r="J125">
+        <v>0</v>
+      </c>
+      <c r="K125">
+        <v>1</v>
+      </c>
+      <c r="L125">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>5</v>
+      </c>
+      <c r="B126" t="s">
+        <v>18</v>
+      </c>
+      <c r="C126" t="s">
+        <v>19</v>
+      </c>
+      <c r="D126" t="s">
+        <v>36</v>
+      </c>
+      <c r="E126">
+        <f>SUM(E124:E125)</f>
+        <v>4</v>
+      </c>
+      <c r="F126">
+        <f t="shared" ref="F126:L126" si="23">SUM(F124:F125)</f>
+        <v>16</v>
+      </c>
+      <c r="G126">
+        <f t="shared" si="23"/>
+        <v>2</v>
+      </c>
+      <c r="H126">
+        <f t="shared" si="23"/>
+        <v>14</v>
+      </c>
+      <c r="I126">
+        <f t="shared" si="23"/>
+        <v>1</v>
+      </c>
+      <c r="J126">
+        <f t="shared" si="23"/>
+        <v>2</v>
+      </c>
+      <c r="K126">
+        <f t="shared" si="23"/>
+        <v>12</v>
+      </c>
+      <c r="L126">
+        <f t="shared" si="23"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>5</v>
+      </c>
+      <c r="B127" t="s">
+        <v>20</v>
+      </c>
+      <c r="C127" t="s">
+        <v>10</v>
+      </c>
+      <c r="D127">
+        <v>1</v>
+      </c>
+      <c r="E127">
+        <v>1</v>
+      </c>
+      <c r="F127">
+        <v>9</v>
+      </c>
+      <c r="G127">
+        <v>7</v>
+      </c>
+      <c r="H127">
+        <f t="shared" si="20"/>
+        <v>2</v>
+      </c>
+      <c r="I127">
+        <v>0</v>
+      </c>
+      <c r="J127">
+        <v>1</v>
+      </c>
+      <c r="K127">
+        <v>1</v>
+      </c>
+      <c r="L127">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>5</v>
+      </c>
+      <c r="B128" t="s">
+        <v>20</v>
+      </c>
+      <c r="C128" t="s">
+        <v>10</v>
+      </c>
+      <c r="D128">
+        <v>2</v>
+      </c>
+      <c r="E128">
+        <v>1</v>
+      </c>
+      <c r="F128">
+        <v>2</v>
+      </c>
+      <c r="G128">
+        <v>0</v>
+      </c>
+      <c r="H128">
+        <f t="shared" si="20"/>
+        <v>2</v>
+      </c>
+      <c r="I128">
+        <v>1</v>
+      </c>
+      <c r="J128">
+        <v>1</v>
+      </c>
+      <c r="K128">
+        <v>0</v>
+      </c>
+      <c r="L128">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>5</v>
+      </c>
+      <c r="B129" t="s">
+        <v>20</v>
+      </c>
+      <c r="C129" t="s">
+        <v>10</v>
+      </c>
+      <c r="D129" t="s">
+        <v>36</v>
+      </c>
+      <c r="E129">
+        <f>SUM(E127:E128)</f>
+        <v>2</v>
+      </c>
+      <c r="F129">
+        <f t="shared" ref="F129:L129" si="24">SUM(F127:F128)</f>
+        <v>11</v>
+      </c>
+      <c r="G129">
+        <f t="shared" si="24"/>
+        <v>7</v>
+      </c>
+      <c r="H129">
+        <f t="shared" si="24"/>
+        <v>4</v>
+      </c>
+      <c r="I129">
+        <f t="shared" si="24"/>
+        <v>1</v>
+      </c>
+      <c r="J129">
+        <f t="shared" si="24"/>
+        <v>2</v>
+      </c>
+      <c r="K129">
+        <f t="shared" si="24"/>
+        <v>1</v>
+      </c>
+      <c r="L129">
+        <f t="shared" si="24"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>5</v>
+      </c>
+      <c r="B130" t="s">
+        <v>21</v>
+      </c>
+      <c r="C130" t="s">
+        <v>10</v>
+      </c>
+      <c r="D130">
+        <v>1</v>
+      </c>
+      <c r="E130">
+        <v>1</v>
+      </c>
+      <c r="F130">
+        <v>10</v>
+      </c>
+      <c r="G130">
+        <v>8</v>
+      </c>
+      <c r="H130">
+        <f t="shared" si="20"/>
+        <v>2</v>
+      </c>
+      <c r="I130">
+        <v>0</v>
+      </c>
+      <c r="J130">
+        <v>1</v>
+      </c>
+      <c r="K130">
+        <v>2</v>
+      </c>
+      <c r="L130">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>5</v>
+      </c>
+      <c r="B131" t="s">
+        <v>21</v>
+      </c>
+      <c r="C131" t="s">
+        <v>10</v>
+      </c>
+      <c r="D131">
+        <v>2</v>
+      </c>
+      <c r="E131">
+        <v>0</v>
+      </c>
+      <c r="F131">
+        <v>3</v>
+      </c>
+      <c r="G131">
+        <v>2</v>
+      </c>
+      <c r="H131">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+      <c r="I131">
+        <v>0</v>
+      </c>
+      <c r="J131">
+        <v>1</v>
+      </c>
+      <c r="K131">
+        <v>1</v>
+      </c>
+      <c r="L131">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>5</v>
+      </c>
+      <c r="B132" t="s">
+        <v>21</v>
+      </c>
+      <c r="C132" t="s">
+        <v>10</v>
+      </c>
+      <c r="D132" t="s">
+        <v>36</v>
+      </c>
+      <c r="E132">
+        <f>SUM(E130:E131)</f>
+        <v>1</v>
+      </c>
+      <c r="F132">
+        <f t="shared" ref="F132:L132" si="25">SUM(F130:F131)</f>
+        <v>13</v>
+      </c>
+      <c r="G132">
+        <f t="shared" si="25"/>
+        <v>10</v>
+      </c>
+      <c r="H132">
+        <f t="shared" si="25"/>
+        <v>3</v>
+      </c>
+      <c r="I132">
+        <f t="shared" si="25"/>
+        <v>0</v>
+      </c>
+      <c r="J132">
+        <f t="shared" si="25"/>
+        <v>2</v>
+      </c>
+      <c r="K132">
+        <f t="shared" si="25"/>
+        <v>3</v>
+      </c>
+      <c r="L132">
+        <f t="shared" si="25"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>5</v>
+      </c>
+      <c r="B133" t="s">
+        <v>22</v>
+      </c>
+      <c r="C133" t="s">
+        <v>19</v>
+      </c>
+      <c r="D133">
+        <v>1</v>
+      </c>
+      <c r="E133">
+        <v>4</v>
+      </c>
+      <c r="F133">
+        <v>12</v>
+      </c>
+      <c r="G133">
+        <v>3</v>
+      </c>
+      <c r="H133">
+        <f t="shared" si="20"/>
+        <v>9</v>
+      </c>
+      <c r="I133">
+        <v>0</v>
+      </c>
+      <c r="J133">
+        <v>5</v>
+      </c>
+      <c r="K133">
+        <v>5</v>
+      </c>
+      <c r="L133">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>5</v>
+      </c>
+      <c r="B134" t="s">
+        <v>22</v>
+      </c>
+      <c r="C134" t="s">
+        <v>19</v>
+      </c>
+      <c r="D134">
+        <v>2</v>
+      </c>
+      <c r="E134">
+        <v>2</v>
+      </c>
+      <c r="F134">
+        <v>12</v>
+      </c>
+      <c r="G134">
+        <v>3</v>
+      </c>
+      <c r="H134">
+        <f t="shared" si="20"/>
+        <v>9</v>
+      </c>
+      <c r="I134">
+        <v>3</v>
+      </c>
+      <c r="J134">
+        <v>4</v>
+      </c>
+      <c r="K134">
+        <v>5</v>
+      </c>
+      <c r="L134">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>5</v>
+      </c>
+      <c r="B135" t="s">
+        <v>22</v>
+      </c>
+      <c r="C135" t="s">
+        <v>19</v>
+      </c>
+      <c r="D135" t="s">
+        <v>36</v>
+      </c>
+      <c r="E135">
+        <f>SUM(E133:E134)</f>
+        <v>6</v>
+      </c>
+      <c r="F135">
+        <f t="shared" ref="F135:L135" si="26">SUM(F133:F134)</f>
+        <v>24</v>
+      </c>
+      <c r="G135">
+        <f t="shared" si="26"/>
+        <v>6</v>
+      </c>
+      <c r="H135">
+        <f t="shared" si="26"/>
+        <v>18</v>
+      </c>
+      <c r="I135">
+        <f t="shared" si="26"/>
+        <v>3</v>
+      </c>
+      <c r="J135">
+        <f t="shared" si="26"/>
+        <v>9</v>
+      </c>
+      <c r="K135">
+        <f t="shared" si="26"/>
+        <v>10</v>
+      </c>
+      <c r="L135">
+        <f t="shared" si="26"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <v>5</v>
+      </c>
+      <c r="B136" t="s">
+        <v>23</v>
+      </c>
+      <c r="C136" t="s">
+        <v>10</v>
+      </c>
+      <c r="D136">
+        <v>1</v>
+      </c>
+      <c r="E136">
+        <v>4</v>
+      </c>
+      <c r="F136">
+        <v>27</v>
+      </c>
+      <c r="G136">
+        <v>17</v>
+      </c>
+      <c r="H136">
+        <f t="shared" si="20"/>
+        <v>10</v>
+      </c>
+      <c r="I136">
+        <v>4</v>
+      </c>
+      <c r="J136">
+        <v>6</v>
+      </c>
+      <c r="K136">
+        <v>2</v>
+      </c>
+      <c r="L136">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>5</v>
+      </c>
+      <c r="B137" t="s">
+        <v>23</v>
+      </c>
+      <c r="C137" t="s">
+        <v>10</v>
+      </c>
+      <c r="D137">
+        <v>2</v>
+      </c>
+      <c r="E137">
+        <v>1</v>
+      </c>
+      <c r="F137">
+        <v>3</v>
+      </c>
+      <c r="G137">
+        <v>2</v>
+      </c>
+      <c r="H137">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+      <c r="I137">
+        <v>0</v>
+      </c>
+      <c r="J137">
+        <v>1</v>
+      </c>
+      <c r="K137">
+        <v>0</v>
+      </c>
+      <c r="L137">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>5</v>
+      </c>
+      <c r="B138" t="s">
+        <v>23</v>
+      </c>
+      <c r="C138" t="s">
+        <v>10</v>
+      </c>
+      <c r="D138" t="s">
+        <v>36</v>
+      </c>
+      <c r="E138">
+        <f>SUM(E136:E137)</f>
+        <v>5</v>
+      </c>
+      <c r="F138">
+        <f t="shared" ref="F138:L138" si="27">SUM(F136:F137)</f>
+        <v>30</v>
+      </c>
+      <c r="G138">
+        <f t="shared" si="27"/>
+        <v>19</v>
+      </c>
+      <c r="H138">
+        <f t="shared" si="27"/>
+        <v>11</v>
+      </c>
+      <c r="I138">
+        <f t="shared" si="27"/>
+        <v>4</v>
+      </c>
+      <c r="J138">
+        <f t="shared" si="27"/>
+        <v>7</v>
+      </c>
+      <c r="K138">
+        <f t="shared" si="27"/>
+        <v>2</v>
+      </c>
+      <c r="L138">
+        <f t="shared" si="27"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>5</v>
+      </c>
+      <c r="B139" t="s">
+        <v>24</v>
+      </c>
+      <c r="C139" t="s">
+        <v>19</v>
+      </c>
+      <c r="D139">
+        <v>1</v>
+      </c>
+      <c r="E139">
+        <v>3</v>
+      </c>
+      <c r="F139">
+        <v>18</v>
+      </c>
+      <c r="G139">
+        <v>12</v>
+      </c>
+      <c r="H139">
+        <f t="shared" si="20"/>
+        <v>6</v>
+      </c>
+      <c r="I139">
+        <v>0</v>
+      </c>
+      <c r="J139">
+        <v>0</v>
+      </c>
+      <c r="K139">
+        <v>2</v>
+      </c>
+      <c r="L139">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <v>5</v>
+      </c>
+      <c r="B140" t="s">
+        <v>24</v>
+      </c>
+      <c r="C140" t="s">
+        <v>19</v>
+      </c>
+      <c r="D140">
+        <v>2</v>
+      </c>
+      <c r="E140">
+        <v>0</v>
+      </c>
+      <c r="F140">
+        <v>4</v>
+      </c>
+      <c r="G140">
+        <v>1</v>
+      </c>
+      <c r="H140">
+        <f t="shared" si="20"/>
+        <v>3</v>
+      </c>
+      <c r="I140">
+        <v>0</v>
+      </c>
+      <c r="J140">
+        <v>2</v>
+      </c>
+      <c r="K140">
+        <v>3</v>
+      </c>
+      <c r="L140">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>5</v>
+      </c>
+      <c r="B141" t="s">
+        <v>24</v>
+      </c>
+      <c r="C141" t="s">
+        <v>19</v>
+      </c>
+      <c r="D141" t="s">
+        <v>36</v>
+      </c>
+      <c r="E141">
+        <f>SUM(E139:E140)</f>
+        <v>3</v>
+      </c>
+      <c r="F141">
+        <f t="shared" ref="F141:L141" si="28">SUM(F139:F140)</f>
+        <v>22</v>
+      </c>
+      <c r="G141">
+        <f t="shared" si="28"/>
+        <v>13</v>
+      </c>
+      <c r="H141">
+        <f t="shared" si="28"/>
+        <v>9</v>
+      </c>
+      <c r="I141">
+        <f t="shared" si="28"/>
+        <v>0</v>
+      </c>
+      <c r="J141">
+        <f t="shared" si="28"/>
+        <v>2</v>
+      </c>
+      <c r="K141">
+        <f t="shared" si="28"/>
+        <v>5</v>
+      </c>
+      <c r="L141">
+        <f t="shared" si="28"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <v>5</v>
+      </c>
+      <c r="B142" t="s">
+        <v>25</v>
+      </c>
+      <c r="C142" t="s">
+        <v>10</v>
+      </c>
+      <c r="D142">
+        <v>1</v>
+      </c>
+      <c r="E142">
+        <v>1</v>
+      </c>
+      <c r="F142">
+        <v>15</v>
+      </c>
+      <c r="G142">
+        <v>7</v>
+      </c>
+      <c r="H142">
+        <f t="shared" si="20"/>
+        <v>8</v>
+      </c>
+      <c r="I142">
+        <v>5</v>
+      </c>
+      <c r="J142">
+        <v>6</v>
+      </c>
+      <c r="K142">
+        <v>2</v>
+      </c>
+      <c r="L142">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <v>5</v>
+      </c>
+      <c r="B143" t="s">
+        <v>25</v>
+      </c>
+      <c r="C143" t="s">
+        <v>10</v>
+      </c>
+      <c r="D143">
+        <v>2</v>
+      </c>
+      <c r="E143">
+        <v>1</v>
+      </c>
+      <c r="F143">
+        <v>6</v>
+      </c>
+      <c r="G143">
+        <v>3</v>
+      </c>
+      <c r="H143">
+        <f t="shared" si="20"/>
+        <v>3</v>
+      </c>
+      <c r="I143">
+        <v>1</v>
+      </c>
+      <c r="J143">
+        <v>1</v>
+      </c>
+      <c r="K143">
+        <v>1</v>
+      </c>
+      <c r="L143">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A144">
+        <v>5</v>
+      </c>
+      <c r="B144" t="s">
+        <v>25</v>
+      </c>
+      <c r="C144" t="s">
+        <v>10</v>
+      </c>
+      <c r="D144" t="s">
+        <v>36</v>
+      </c>
+      <c r="E144">
+        <f>SUM(E142:E143)</f>
+        <v>2</v>
+      </c>
+      <c r="F144">
+        <f t="shared" ref="F144:L144" si="29">SUM(F142:F143)</f>
+        <v>21</v>
+      </c>
+      <c r="G144">
+        <f t="shared" si="29"/>
+        <v>10</v>
+      </c>
+      <c r="H144">
+        <f t="shared" si="29"/>
+        <v>11</v>
+      </c>
+      <c r="I144">
+        <f t="shared" si="29"/>
+        <v>6</v>
+      </c>
+      <c r="J144">
+        <f t="shared" si="29"/>
+        <v>7</v>
+      </c>
+      <c r="K144">
+        <f t="shared" si="29"/>
+        <v>3</v>
+      </c>
+      <c r="L144">
+        <f t="shared" si="29"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="145" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <v>5</v>
+      </c>
+      <c r="B145" t="s">
+        <v>30</v>
+      </c>
+      <c r="C145" t="s">
+        <v>19</v>
+      </c>
+      <c r="D145">
+        <v>1</v>
+      </c>
+      <c r="E145">
+        <v>3</v>
+      </c>
+      <c r="F145">
+        <v>31</v>
+      </c>
+      <c r="G145">
+        <v>18</v>
+      </c>
+      <c r="H145">
+        <f t="shared" si="20"/>
+        <v>13</v>
+      </c>
+      <c r="I145">
+        <v>3</v>
+      </c>
+      <c r="J145">
+        <v>7</v>
+      </c>
+      <c r="K145">
+        <v>7</v>
+      </c>
+      <c r="L145">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="146" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A146">
+        <v>5</v>
+      </c>
+      <c r="B146" t="s">
+        <v>30</v>
+      </c>
+      <c r="C146" t="s">
+        <v>19</v>
+      </c>
+      <c r="D146">
+        <v>2</v>
+      </c>
+      <c r="E146">
+        <v>0</v>
+      </c>
+      <c r="F146">
+        <v>3</v>
+      </c>
+      <c r="G146">
+        <v>2</v>
+      </c>
+      <c r="H146">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+      <c r="I146">
+        <v>0</v>
+      </c>
+      <c r="J146">
+        <v>1</v>
+      </c>
+      <c r="K146">
+        <v>1</v>
+      </c>
+      <c r="L146">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A147">
+        <v>5</v>
+      </c>
+      <c r="B147" t="s">
+        <v>30</v>
+      </c>
+      <c r="C147" t="s">
+        <v>19</v>
+      </c>
+      <c r="D147" t="s">
+        <v>36</v>
+      </c>
+      <c r="E147">
+        <f>SUM(E145:E146)</f>
+        <v>3</v>
+      </c>
+      <c r="F147">
+        <f t="shared" ref="F147:L147" si="30">SUM(F145:F146)</f>
+        <v>34</v>
+      </c>
+      <c r="G147">
+        <f t="shared" si="30"/>
+        <v>20</v>
+      </c>
+      <c r="H147">
+        <f t="shared" si="30"/>
+        <v>14</v>
+      </c>
+      <c r="I147">
+        <f t="shared" si="30"/>
+        <v>3</v>
+      </c>
+      <c r="J147">
+        <f t="shared" si="30"/>
+        <v>8</v>
+      </c>
+      <c r="K147">
+        <f t="shared" si="30"/>
+        <v>8</v>
+      </c>
+      <c r="L147">
+        <f t="shared" si="30"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="148" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A148">
+        <v>5</v>
+      </c>
+      <c r="B148" t="s">
+        <v>26</v>
+      </c>
+      <c r="C148" t="s">
+        <v>19</v>
+      </c>
+      <c r="D148">
+        <v>1</v>
+      </c>
+      <c r="E148">
+        <v>2</v>
+      </c>
+      <c r="F148">
+        <v>20</v>
+      </c>
+      <c r="G148">
+        <v>13</v>
+      </c>
+      <c r="H148">
+        <f t="shared" si="20"/>
+        <v>7</v>
+      </c>
+      <c r="I148">
+        <v>4</v>
+      </c>
+      <c r="J148">
+        <v>4</v>
+      </c>
+      <c r="K148">
+        <v>1</v>
+      </c>
+      <c r="L148">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="149" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A149">
+        <v>5</v>
+      </c>
+      <c r="B149" t="s">
+        <v>26</v>
+      </c>
+      <c r="C149" t="s">
+        <v>19</v>
+      </c>
+      <c r="D149">
+        <v>2</v>
+      </c>
+      <c r="E149">
+        <v>1</v>
+      </c>
+      <c r="F149">
+        <v>1</v>
+      </c>
+      <c r="G149">
+        <v>0</v>
+      </c>
+      <c r="H149">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+      <c r="I149">
+        <v>0</v>
+      </c>
+      <c r="J149">
+        <v>1</v>
+      </c>
+      <c r="K149">
+        <v>0</v>
+      </c>
+      <c r="L149">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A150">
+        <v>5</v>
+      </c>
+      <c r="B150" t="s">
+        <v>26</v>
+      </c>
+      <c r="C150" t="s">
+        <v>19</v>
+      </c>
+      <c r="D150" t="s">
+        <v>36</v>
+      </c>
+      <c r="E150">
+        <f>SUM(E148:E149)</f>
+        <v>3</v>
+      </c>
+      <c r="F150">
+        <f t="shared" ref="F150:L150" si="31">SUM(F148:F149)</f>
+        <v>21</v>
+      </c>
+      <c r="G150">
+        <f t="shared" si="31"/>
+        <v>13</v>
+      </c>
+      <c r="H150">
+        <f t="shared" si="31"/>
+        <v>8</v>
+      </c>
+      <c r="I150">
+        <f t="shared" si="31"/>
+        <v>4</v>
+      </c>
+      <c r="J150">
+        <f t="shared" si="31"/>
+        <v>5</v>
+      </c>
+      <c r="K150">
+        <f t="shared" si="31"/>
+        <v>1</v>
+      </c>
+      <c r="L150">
+        <f t="shared" si="31"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="151" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A151">
+        <v>5</v>
+      </c>
+      <c r="B151" t="s">
+        <v>27</v>
+      </c>
+      <c r="C151" t="s">
+        <v>10</v>
+      </c>
+      <c r="D151">
+        <v>1</v>
+      </c>
+      <c r="E151">
+        <v>2</v>
+      </c>
+      <c r="F151">
+        <v>5</v>
+      </c>
+      <c r="G151">
+        <v>3</v>
+      </c>
+      <c r="H151">
+        <f t="shared" si="20"/>
+        <v>2</v>
+      </c>
+      <c r="I151">
+        <v>0</v>
+      </c>
+      <c r="J151">
+        <v>0</v>
+      </c>
+      <c r="K151">
+        <v>0</v>
+      </c>
+      <c r="L151">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="152" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A152">
+        <v>5</v>
+      </c>
+      <c r="B152" t="s">
+        <v>27</v>
+      </c>
+      <c r="C152" t="s">
+        <v>10</v>
+      </c>
+      <c r="D152">
+        <v>2</v>
+      </c>
+      <c r="E152">
+        <v>0</v>
+      </c>
+      <c r="F152">
+        <v>7</v>
+      </c>
+      <c r="G152">
+        <v>4</v>
+      </c>
+      <c r="H152">
+        <f t="shared" si="20"/>
+        <v>3</v>
+      </c>
+      <c r="I152">
+        <v>0</v>
+      </c>
+      <c r="J152">
+        <v>1</v>
+      </c>
+      <c r="K152">
+        <v>3</v>
+      </c>
+      <c r="L152">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="153" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A153">
+        <v>5</v>
+      </c>
+      <c r="B153" t="s">
+        <v>27</v>
+      </c>
+      <c r="C153" t="s">
+        <v>10</v>
+      </c>
+      <c r="D153" t="s">
+        <v>36</v>
+      </c>
+      <c r="E153">
+        <f>SUM(E151:E152)</f>
+        <v>2</v>
+      </c>
+      <c r="F153">
+        <f t="shared" ref="F153:L153" si="32">SUM(F151:F152)</f>
+        <v>12</v>
+      </c>
+      <c r="G153">
+        <f t="shared" si="32"/>
+        <v>7</v>
+      </c>
+      <c r="H153">
+        <f t="shared" si="32"/>
+        <v>5</v>
+      </c>
+      <c r="I153">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="J153">
+        <f t="shared" si="32"/>
+        <v>1</v>
+      </c>
+      <c r="K153">
+        <f t="shared" si="32"/>
+        <v>3</v>
+      </c>
+      <c r="L153">
+        <f t="shared" si="32"/>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Small changes? Moved things around folders
</commit_message>
<xml_diff>
--- a/data/combined_individual_data.xlsx
+++ b/data/combined_individual_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janya\Desktop\R\bb_soc_exp\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4065E8F-C1F6-467B-A04D-4601054CFA88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24481C72-2EF9-4308-AF6D-7110F6DE6F4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -188,9 +188,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -474,8 +473,8 @@
   <dimension ref="A1:R189"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A151" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P162" sqref="P162"/>
+      <pane ySplit="1" topLeftCell="A112" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C121" sqref="C121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6177,7 +6176,7 @@
         <v>11</v>
       </c>
       <c r="C118" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="D118">
         <v>1</v>
@@ -6216,7 +6215,7 @@
         <v>11</v>
       </c>
       <c r="C119" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="D119">
         <v>2</v>
@@ -6231,7 +6230,7 @@
         <v>0</v>
       </c>
       <c r="H119">
-        <f t="shared" ref="H119:H162" si="20">F119-G119</f>
+        <f t="shared" ref="H119:H152" si="20">F119-G119</f>
         <v>3</v>
       </c>
       <c r="I119">
@@ -6255,7 +6254,7 @@
         <v>11</v>
       </c>
       <c r="C120" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="D120" t="s">
         <v>36</v>
@@ -7679,11 +7678,11 @@
       <c r="G154">
         <v>0</v>
       </c>
-      <c r="H154" s="1">
+      <c r="H154">
         <f>F154-G154</f>
         <v>2</v>
       </c>
-      <c r="I154" s="1">
+      <c r="I154">
         <v>0</v>
       </c>
       <c r="J154">
@@ -7719,19 +7718,19 @@
         <v>1</v>
       </c>
       <c r="H155">
-        <f t="shared" ref="H155:H189" si="33">F155-G155</f>
-        <v>1</v>
-      </c>
-      <c r="I155" s="1">
-        <v>0</v>
-      </c>
-      <c r="J155" s="1">
-        <v>0</v>
-      </c>
-      <c r="K155" s="1">
-        <v>1</v>
-      </c>
-      <c r="L155" s="1">
+        <f t="shared" ref="H155:H188" si="33">F155-G155</f>
+        <v>1</v>
+      </c>
+      <c r="I155">
+        <v>0</v>
+      </c>
+      <c r="J155">
+        <v>0</v>
+      </c>
+      <c r="K155">
+        <v>1</v>
+      </c>
+      <c r="L155">
         <v>1</v>
       </c>
     </row>

</xml_diff>